<commit_message>
Bumped version number to 5.1
Former-commit-id: 87a90f4fca8246e967d27ceb368056860373330c [formerly d49161df9969e83f472691c55796347ca747bd66]
Former-commit-id: 368ca17c4831a1e30706be4c7001cb628c87c04e
</commit_message>
<xml_diff>
--- a/public/port-battle.xlsx
+++ b/public/port-battle.xlsx
@@ -1363,7 +1363,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFE192B6"/>
+      <color rgb="FFDEAEC4"/>
       <name val="Calibri"/>
       <family val="1"/>
       <b/>
@@ -1383,7 +1383,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF79B0EA"/>
+      <color rgb="FFA2C1E3"/>
       <name val="Calibri"/>
       <family val="1"/>
       <b/>
@@ -1459,10 +1459,10 @@
       <left/>
       <right/>
       <top style="thin">
-        <color rgb="FFC6C5C5"/>
+        <color rgb="FFC5C3C3"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C5C5"/>
+        <color rgb="FFC5C3C3"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1550,7 +1550,7 @@
     <dxf>
       <font>
         <sz val="12"/>
-        <color rgb="FFE192B6"/>
+        <color rgb="FFDEAEC4"/>
         <name val="Calibri"/>
         <family val="1"/>
         <b/>

</xml_diff>

<commit_message>
Bumped version number to 5.3
Former-commit-id: 428188869fbd8b4e1543585248dbf01cd497ad19 [formerly 0598420d59fb91257a91429ef30652520278dd27]
Former-commit-id: cbe1073f0404bc35114a2d456382aeee216d4a45
</commit_message>
<xml_diff>
--- a/public/port-battle.xlsx
+++ b/public/port-battle.xlsx
@@ -140,13 +140,13 @@
     <t>Cerberus</t>
   </si>
   <si>
+    <t>Hercules</t>
+  </si>
+  <si>
+    <t>Pandora</t>
+  </si>
+  <si>
     <t>Le Requin</t>
-  </si>
-  <si>
-    <t>Pandora</t>
-  </si>
-  <si>
-    <t>Hercules</t>
   </si>
   <si>
     <t>Mercury</t>
@@ -3210,7 +3210,7 @@
         <v>42</v>
       </c>
       <c r="C35" s="27" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D35" s="27">
         <f>COUNTA(F35:AC35)</f>

</xml_diff>

<commit_message>
Bumped version number to 7
Former-commit-id: ab818f81584d76d62d7c0e67b0b0f557de10b260
</commit_message>
<xml_diff>
--- a/public/port-battle.xlsx
+++ b/public/port-battle.xlsx
@@ -59,10 +59,10 @@
     <t>Victory</t>
   </si>
   <si>
+    <t>Bucentaure</t>
+  </si>
+  <si>
     <t>Christian</t>
-  </si>
-  <si>
-    <t>Bucentaure</t>
   </si>
   <si>
     <t>St. Pavel</t>
@@ -1947,7 +1947,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="32" t="n">
-        <v>500</v>
+        <v>460</v>
       </c>
       <c r="D8" s="32">
         <f>COUNTA(F8:AC8)</f>
@@ -1994,7 +1994,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="32" t="n">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="D9" s="32">
         <f>COUNTA(F9:AC9)</f>

</xml_diff>